<commit_message>
it works well enough
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cass4\Documents\ML\ANNDigitRecognition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E6BD3F-8E42-4667-BB2A-F0C39F140763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34443BEE-3418-4CE5-9214-A1B3E0191905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{BFAD6376-658E-4557-9510-7FF7B0FC0418}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="16120" windowHeight="9190" xr2:uid="{BFAD6376-658E-4557-9510-7FF7B0FC0418}"/>
   </bookViews>
   <sheets>
-    <sheet name="X" sheetId="1" r:id="rId1"/>
-    <sheet name="data" sheetId="3" r:id="rId2"/>
-    <sheet name="Y" sheetId="2" r:id="rId3"/>
+    <sheet name="x_train" sheetId="4" r:id="rId1"/>
+    <sheet name="y_train" sheetId="5" r:id="rId2"/>
+    <sheet name="x_test" sheetId="1" r:id="rId3"/>
+    <sheet name="y_test" sheetId="2" r:id="rId4"/>
+    <sheet name="data" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -382,11 +384,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56EFBFB9-E802-4C6D-8733-9A2BF8122C01}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7D4EEBA-62D3-4518-B4EA-02030212AF9F}">
   <dimension ref="A1:AS40"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="X40" sqref="A1:AS40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -751,10 +753,10 @@
         <v>0</v>
       </c>
       <c r="AC3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE3">
         <v>0</v>
@@ -766,10 +768,10 @@
         <v>0</v>
       </c>
       <c r="AH3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ3">
         <v>1</v>
@@ -5877,10 +5879,3025 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB260DAA-2E06-44B1-907A-EAA77BA619A3}">
+  <dimension ref="A1:J40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:J40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
+      </c>
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1">
+        <v>0</v>
+      </c>
+      <c r="H1">
+        <v>0</v>
+      </c>
+      <c r="I1">
+        <v>0</v>
+      </c>
+      <c r="J1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>0</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>0</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>0</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56EFBFB9-E802-4C6D-8733-9A2BF8122C01}">
+  <dimension ref="A1:AS10"/>
+  <sheetViews>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
+      </c>
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1">
+        <v>1</v>
+      </c>
+      <c r="H1">
+        <v>1</v>
+      </c>
+      <c r="I1">
+        <v>1</v>
+      </c>
+      <c r="J1">
+        <v>0</v>
+      </c>
+      <c r="K1">
+        <v>1</v>
+      </c>
+      <c r="L1">
+        <v>0</v>
+      </c>
+      <c r="M1">
+        <v>1</v>
+      </c>
+      <c r="N1">
+        <v>0</v>
+      </c>
+      <c r="O1">
+        <v>0</v>
+      </c>
+      <c r="P1">
+        <v>0</v>
+      </c>
+      <c r="Q1">
+        <v>0</v>
+      </c>
+      <c r="R1">
+        <v>1</v>
+      </c>
+      <c r="S1">
+        <v>0</v>
+      </c>
+      <c r="T1">
+        <v>0</v>
+      </c>
+      <c r="U1">
+        <v>0</v>
+      </c>
+      <c r="V1">
+        <v>0</v>
+      </c>
+      <c r="W1">
+        <v>1</v>
+      </c>
+      <c r="X1">
+        <v>0</v>
+      </c>
+      <c r="Y1">
+        <v>0</v>
+      </c>
+      <c r="Z1">
+        <v>0</v>
+      </c>
+      <c r="AA1">
+        <v>0</v>
+      </c>
+      <c r="AB1">
+        <v>1</v>
+      </c>
+      <c r="AC1">
+        <v>0</v>
+      </c>
+      <c r="AD1">
+        <v>0</v>
+      </c>
+      <c r="AE1">
+        <v>0</v>
+      </c>
+      <c r="AF1">
+        <v>0</v>
+      </c>
+      <c r="AG1">
+        <v>1</v>
+      </c>
+      <c r="AH1">
+        <v>0</v>
+      </c>
+      <c r="AI1">
+        <v>0</v>
+      </c>
+      <c r="AJ1">
+        <v>0</v>
+      </c>
+      <c r="AK1">
+        <v>0</v>
+      </c>
+      <c r="AL1">
+        <v>1</v>
+      </c>
+      <c r="AM1">
+        <v>0</v>
+      </c>
+      <c r="AN1">
+        <v>0</v>
+      </c>
+      <c r="AO1">
+        <v>0</v>
+      </c>
+      <c r="AP1">
+        <v>0</v>
+      </c>
+      <c r="AQ1">
+        <v>1</v>
+      </c>
+      <c r="AR1">
+        <v>0</v>
+      </c>
+      <c r="AS1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>1</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>1</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>1</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>1</v>
+      </c>
+      <c r="AP2">
+        <v>1</v>
+      </c>
+      <c r="AQ2">
+        <v>1</v>
+      </c>
+      <c r="AR2">
+        <v>1</v>
+      </c>
+      <c r="AS2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>1</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>1</v>
+      </c>
+      <c r="AK3">
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3">
+        <v>1</v>
+      </c>
+      <c r="AP3">
+        <v>1</v>
+      </c>
+      <c r="AQ3">
+        <v>1</v>
+      </c>
+      <c r="AR3">
+        <v>1</v>
+      </c>
+      <c r="AS3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>1</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>1</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>1</v>
+      </c>
+      <c r="AF4">
+        <v>1</v>
+      </c>
+      <c r="AG4">
+        <v>1</v>
+      </c>
+      <c r="AH4">
+        <v>1</v>
+      </c>
+      <c r="AI4">
+        <v>1</v>
+      </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>1</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <v>0</v>
+      </c>
+      <c r="AP4">
+        <v>0</v>
+      </c>
+      <c r="AQ4">
+        <v>0</v>
+      </c>
+      <c r="AR4">
+        <v>1</v>
+      </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>1</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
+        <v>1</v>
+      </c>
+      <c r="AJ5">
+        <v>1</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <v>1</v>
+      </c>
+      <c r="AO5">
+        <v>0</v>
+      </c>
+      <c r="AP5">
+        <v>1</v>
+      </c>
+      <c r="AQ5">
+        <v>1</v>
+      </c>
+      <c r="AR5">
+        <v>1</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>1</v>
+      </c>
+      <c r="AE6">
+        <v>1</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <v>1</v>
+      </c>
+      <c r="AJ6">
+        <v>1</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AN6">
+        <v>1</v>
+      </c>
+      <c r="AO6">
+        <v>0</v>
+      </c>
+      <c r="AP6">
+        <v>1</v>
+      </c>
+      <c r="AQ6">
+        <v>1</v>
+      </c>
+      <c r="AR6">
+        <v>1</v>
+      </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>1</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>1</v>
+      </c>
+      <c r="AG7">
+        <v>0</v>
+      </c>
+      <c r="AH7">
+        <v>0</v>
+      </c>
+      <c r="AI7">
+        <v>0</v>
+      </c>
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+      <c r="AK7">
+        <v>1</v>
+      </c>
+      <c r="AL7">
+        <v>0</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>0</v>
+      </c>
+      <c r="AP7">
+        <v>1</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
+      <c r="AR7">
+        <v>0</v>
+      </c>
+      <c r="AS7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>1</v>
+      </c>
+      <c r="AE8">
+        <v>1</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
+        <v>1</v>
+      </c>
+      <c r="AJ8">
+        <v>1</v>
+      </c>
+      <c r="AK8">
+        <v>0</v>
+      </c>
+      <c r="AL8">
+        <v>0</v>
+      </c>
+      <c r="AM8">
+        <v>0</v>
+      </c>
+      <c r="AN8">
+        <v>1</v>
+      </c>
+      <c r="AO8">
+        <v>0</v>
+      </c>
+      <c r="AP8">
+        <v>1</v>
+      </c>
+      <c r="AQ8">
+        <v>1</v>
+      </c>
+      <c r="AR8">
+        <v>1</v>
+      </c>
+      <c r="AS8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>1</v>
+      </c>
+      <c r="W9">
+        <v>1</v>
+      </c>
+      <c r="X9">
+        <v>1</v>
+      </c>
+      <c r="Y9">
+        <v>1</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>1</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>0</v>
+      </c>
+      <c r="AH9">
+        <v>0</v>
+      </c>
+      <c r="AI9">
+        <v>1</v>
+      </c>
+      <c r="AJ9">
+        <v>1</v>
+      </c>
+      <c r="AK9">
+        <v>1</v>
+      </c>
+      <c r="AL9">
+        <v>0</v>
+      </c>
+      <c r="AM9">
+        <v>0</v>
+      </c>
+      <c r="AN9">
+        <v>0</v>
+      </c>
+      <c r="AO9">
+        <v>0</v>
+      </c>
+      <c r="AP9">
+        <v>0</v>
+      </c>
+      <c r="AQ9">
+        <v>0</v>
+      </c>
+      <c r="AR9">
+        <v>1</v>
+      </c>
+      <c r="AS9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>1</v>
+      </c>
+      <c r="Z10">
+        <v>1</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>1</v>
+      </c>
+      <c r="AE10">
+        <v>1</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AG10">
+        <v>0</v>
+      </c>
+      <c r="AH10">
+        <v>0</v>
+      </c>
+      <c r="AI10">
+        <v>1</v>
+      </c>
+      <c r="AJ10">
+        <v>1</v>
+      </c>
+      <c r="AK10">
+        <v>0</v>
+      </c>
+      <c r="AL10">
+        <v>0</v>
+      </c>
+      <c r="AM10">
+        <v>0</v>
+      </c>
+      <c r="AN10">
+        <v>1</v>
+      </c>
+      <c r="AO10">
+        <v>0</v>
+      </c>
+      <c r="AP10">
+        <v>1</v>
+      </c>
+      <c r="AQ10">
+        <v>1</v>
+      </c>
+      <c r="AR10">
+        <v>1</v>
+      </c>
+      <c r="AS10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B69F78F7-8E38-4252-AFF2-4F5E37477485}">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
+      </c>
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1">
+        <v>0</v>
+      </c>
+      <c r="H1">
+        <v>0</v>
+      </c>
+      <c r="I1">
+        <v>0</v>
+      </c>
+      <c r="J1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D9B2BA-10F4-415A-AB1A-8B2247EAA667}">
   <dimension ref="A1:AT40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+    <sheetView topLeftCell="AE1" workbookViewId="0">
       <selection activeCell="AV8" sqref="AV8"/>
     </sheetView>
   </sheetViews>
@@ -11489,219 +14506,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B69F78F7-8E38-4252-AFF2-4F5E37477485}">
-  <dimension ref="A1:A40"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>